<commit_message>
REST API CRUD - start
</commit_message>
<xml_diff>
--- a/Additional Data.xlsx
+++ b/Additional Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\dev\MyAppLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECBE2F8-5AF4-47F6-A58D-E4423BA012F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EBA75F-777D-4118-8C87-168912399886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-8205" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dependencies" sheetId="1" r:id="rId1"/>
+    <sheet name="Dependencies (Dev)" sheetId="2" r:id="rId1"/>
+    <sheet name="Dependencies (Prod)" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>#</t>
   </si>
@@ -45,13 +46,31 @@
     <t>https://www.npmjs.com/package/morgan</t>
   </si>
   <si>
-    <t>morgan</t>
-  </si>
-  <si>
     <t>Uso los middlewaves para varias cosas</t>
   </si>
   <si>
-    <t>npm i morgan --save-dev</t>
+    <t>Express</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Nodemon</t>
+  </si>
+  <si>
+    <t>npm i nodemon --save-dev</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/express</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/nodemon</t>
+  </si>
+  <si>
+    <t>npm i express --save</t>
+  </si>
+  <si>
+    <t>npm i morgan --save</t>
   </si>
 </sst>
 </file>
@@ -116,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -131,6 +150,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -413,18 +435,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C812A21-A379-4664-9F38-3271EC4EAA18}">
   <dimension ref="C2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" style="1"/>
     <col min="3" max="3" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -448,27 +470,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="4">
         <v>2</v>
       </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
@@ -482,9 +502,99 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{9C6C98D1-164A-4C83-8A7A-71B2524A25C1}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{910C72FF-0BE7-424D-89FA-9DF0587C439C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C2:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" style="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="2.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{9C6C98D1-164A-4C83-8A7A-71B2524A25C1}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{AC7AE18C-B3A4-4372-A571-9E6A4076B159}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add postgres, add dependencie (morgan, pg, sequelize, sequelize-cli)
</commit_message>
<xml_diff>
--- a/Additional Data.xlsx
+++ b/Additional Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\dev\MyAppLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EBA75F-777D-4118-8C87-168912399886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F74E31-6341-4566-906A-156FDDE5FB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-8205" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dependencies (Dev)" sheetId="2" r:id="rId1"/>
-    <sheet name="Dependencies (Prod)" sheetId="1" r:id="rId2"/>
+    <sheet name="Dependencies (Prod)" sheetId="1" r:id="rId1"/>
+    <sheet name="Dependencies (Dev)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -71,6 +71,45 @@
   </si>
   <si>
     <t>npm i morgan --save</t>
+  </si>
+  <si>
+    <t>npm i pg --save</t>
+  </si>
+  <si>
+    <t>npm i sequelize  --save</t>
+  </si>
+  <si>
+    <t>npm i sequelize-cli --save</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>sequelize</t>
+  </si>
+  <si>
+    <t>sequelize-cli</t>
+  </si>
+  <si>
+    <t>controlador para usar postgres</t>
+  </si>
+  <si>
+    <t>ORM para node</t>
+  </si>
+  <si>
+    <t>tool command line para sequelize</t>
+  </si>
+  <si>
+    <t>https://sequelize.org/</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/pg</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/sequelize-cli</t>
+  </si>
+  <si>
+    <t>Sirve para editar el codigo y auto ejecutar server</t>
   </si>
 </sst>
 </file>
@@ -435,19 +474,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C812A21-A379-4664-9F38-3271EC4EAA18}">
-  <dimension ref="C2:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" style="1"/>
     <col min="3" max="3" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="2.85546875" style="1"/>
@@ -471,60 +510,100 @@
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="4">
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="4">
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="4">
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{910C72FF-0BE7-424D-89FA-9DF0587C439C}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{9C6C98D1-164A-4C83-8A7A-71B2524A25C1}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{AC7AE18C-B3A4-4372-A571-9E6A4076B159}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{6044C4F7-393F-4DB3-BDA4-DB9367F5A1AA}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{A922C4B9-8470-4AC3-87C8-9D3FB656B017}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C812A21-A379-4664-9F38-3271EC4EAA18}">
+  <dimension ref="C2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" style="1"/>
     <col min="3" max="3" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="2.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -545,54 +624,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="3:7" ht="105" x14ac:dyDescent="0.25">
       <c r="C4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{9C6C98D1-164A-4C83-8A7A-71B2524A25C1}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{AC7AE18C-B3A4-4372-A571-9E6A4076B159}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{910C72FF-0BE7-424D-89FA-9DF0587C439C}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{5D9FF932-0F3B-4A79-B15C-8CBE6B3EB9F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Confg server, add news dependencie (mysql2)
</commit_message>
<xml_diff>
--- a/Additional Data.xlsx
+++ b/Additional Data.xlsx
@@ -8,18 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\dev\MyAppLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F74E31-6341-4566-906A-156FDDE5FB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CB59A5-91EF-47C6-864A-040E4A5F4D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-8205" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-8205" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dependencies (Prod)" sheetId="1" r:id="rId1"/>
     <sheet name="Dependencies (Dev)" sheetId="2" r:id="rId2"/>
+    <sheet name="DataBase" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -174,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -592,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C812A21-A379-4664-9F38-3271EC4EAA18}">
   <dimension ref="C2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
@@ -676,4 +689,23 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D3CAD6-FADA-4897-9A41-A98553E006C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" style="7"/>
+    <col min="3" max="3" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>